<commit_message>
Changes in stock module
</commit_message>
<xml_diff>
--- a/ExcelFiles/StockDomain.xlsx
+++ b/ExcelFiles/StockDomain.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Riomed\DemoServerAutomation\Cellma4Automation\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE30AE1-C558-4F1D-B3A7-55A01A5281B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63AE1A7-15FE-4264-B96C-B2ABEE801AEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="3420" windowWidth="18000" windowHeight="9360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -296,7 +296,7 @@
     <t>TestBatch</t>
   </si>
   <si>
-    <t>Dolo 42 MG</t>
+    <t>Dolo 43 MG</t>
   </si>
 </sst>
 </file>
@@ -744,7 +744,7 @@
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,7 +1018,7 @@
     <row r="2" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="str">
         <f>AddNewStock!A2</f>
-        <v>Dolo 42 MG</v>
+        <v>Dolo 43 MG</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>

</xml_diff>